<commit_message>
Sorted the regex, even though it's a mess...
Muddled through.
</commit_message>
<xml_diff>
--- a/regex_cases_logic.xlsx
+++ b/regex_cases_logic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthew.mcfahn/Documents/GitHub/who-api-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6934CC-92BC-B746-8D53-D6892053ADC0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41DD948A-E9E8-C945-AE2B-F6083F988010}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11680" yWindow="4020" windowWidth="23440" windowHeight="14200" xr2:uid="{D1EB1906-1AF6-C14E-A441-E2525BF29D30}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="20">
   <si>
     <t>Cases</t>
   </si>
@@ -75,25 +75,25 @@
     <t>Need to review cases like</t>
   </si>
   <si>
-    <t>&lt;500 [&lt;500–710]</t>
-  </si>
-  <si>
-    <t>Matches to 6???</t>
-  </si>
-  <si>
-    <t>&lt;500 [&lt;500–&lt;500]</t>
-  </si>
-  <si>
-    <t>Cases 13, 14 - They're fucked…</t>
-  </si>
-  <si>
-    <t>Case15 - Grabbing too many…</t>
-  </si>
-  <si>
     <t>Case 20, 21 also messing up…</t>
   </si>
   <si>
-    <t>LOOKS LIKE MY REGEX ISN'T GREAT :(</t>
+    <t>Just 2,000,000/8,000,000 (double comma) which needs sorting. Maybe as a new coding?</t>
+  </si>
+  <si>
+    <t>TODO:</t>
+  </si>
+  <si>
+    <t>Handle double commas in case 14 (or as a workaround in case 22, then add)</t>
+  </si>
+  <si>
+    <t>Sort out 20, 21 - the regex is crap</t>
+  </si>
+  <si>
+    <t>[330 000-370 000]</t>
+  </si>
+  <si>
+    <t>These cases</t>
   </si>
 </sst>
 </file>
@@ -471,15 +471,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A9C09BF-1A38-5B41-9714-1AF4B5C2B4FD}">
-  <dimension ref="B1:J14"/>
+  <dimension ref="B1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.2">
       <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
@@ -489,7 +489,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -509,7 +509,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>1</v>
       </c>
@@ -529,7 +529,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>2</v>
       </c>
@@ -549,7 +549,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>3</v>
       </c>
@@ -566,7 +566,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>5</v>
       </c>
@@ -586,7 +586,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>6</v>
       </c>
@@ -602,14 +602,8 @@
       <c r="G7" t="s">
         <v>5</v>
       </c>
-      <c r="I7" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>7</v>
       </c>
@@ -625,14 +619,8 @@
       <c r="G8" t="s">
         <v>5</v>
       </c>
-      <c r="I8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>8</v>
       </c>
@@ -648,11 +636,8 @@
       <c r="F9" t="s">
         <v>5</v>
       </c>
-      <c r="I9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>9</v>
       </c>
@@ -672,10 +657,10 @@
         <v>6</v>
       </c>
       <c r="I10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>10</v>
       </c>
@@ -689,55 +674,187 @@
         <v>5</v>
       </c>
       <c r="I11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>14</v>
+      </c>
+      <c r="I14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>20</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12">
-        <v>13</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-      <c r="E12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13">
-        <v>14</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="J17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14">
-        <v>15</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G14" t="s">
-        <v>5</v>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>21</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>22</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>23</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some updates to set up for finishing the regex updating
</commit_message>
<xml_diff>
--- a/regex_cases_logic.xlsx
+++ b/regex_cases_logic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthew.mcfahn/Documents/GitHub/who-api-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41DD948A-E9E8-C945-AE2B-F6083F988010}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE63659F-AE81-E746-ABC5-BF779646A361}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11680" yWindow="4020" windowWidth="23440" windowHeight="14200" xr2:uid="{D1EB1906-1AF6-C14E-A441-E2525BF29D30}"/>
+    <workbookView xWindow="20400" yWindow="4020" windowWidth="14720" windowHeight="14200" xr2:uid="{D1EB1906-1AF6-C14E-A441-E2525BF29D30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="13">
   <si>
     <t>Cases</t>
   </si>
@@ -72,28 +72,7 @@
     <t>Logic is that 'NumX' is the Xth appearing in the string, from the left</t>
   </si>
   <si>
-    <t>Need to review cases like</t>
-  </si>
-  <si>
-    <t>Case 20, 21 also messing up…</t>
-  </si>
-  <si>
-    <t>Just 2,000,000/8,000,000 (double comma) which needs sorting. Maybe as a new coding?</t>
-  </si>
-  <si>
-    <t>TODO:</t>
-  </si>
-  <si>
-    <t>Handle double commas in case 14 (or as a workaround in case 22, then add)</t>
-  </si>
-  <si>
-    <t>Sort out 20, 21 - the regex is crap</t>
-  </si>
-  <si>
-    <t>[330 000-370 000]</t>
-  </si>
-  <si>
-    <t>These cases</t>
+    <t>ApplicationGroup</t>
   </si>
 </sst>
 </file>
@@ -471,15 +450,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A9C09BF-1A38-5B41-9714-1AF4B5C2B4FD}">
-  <dimension ref="B1:J20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
@@ -489,9 +468,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -509,7 +491,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
       <c r="B3">
         <v>1</v>
       </c>
@@ -529,7 +514,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
       <c r="B4">
         <v>2</v>
       </c>
@@ -549,7 +537,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
       <c r="B5">
         <v>3</v>
       </c>
@@ -566,9 +557,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
       <c r="B6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -582,13 +576,13 @@
       <c r="F6" t="s">
         <v>5</v>
       </c>
-      <c r="I6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
       <c r="B7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -603,9 +597,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
       <c r="B8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -620,9 +617,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
       <c r="B9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -637,9 +637,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
       <c r="B10">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -656,13 +659,13 @@
       <c r="G10" t="s">
         <v>6</v>
       </c>
-      <c r="I10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
       <c r="B11">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -673,13 +676,13 @@
       <c r="E11" t="s">
         <v>5</v>
       </c>
-      <c r="I11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
       <c r="B12">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -697,9 +700,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>13</v>
+      </c>
       <c r="B13">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -717,17 +723,35 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>14</v>
+      </c>
       <c r="B14">
-        <v>14</v>
-      </c>
-      <c r="I14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -744,13 +768,13 @@
       <c r="G15" t="s">
         <v>5</v>
       </c>
-      <c r="I15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>19</v>
+      </c>
       <c r="B16">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -767,13 +791,13 @@
       <c r="G16" t="s">
         <v>6</v>
       </c>
-      <c r="I16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>20</v>
+      </c>
       <c r="B17">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -790,16 +814,13 @@
       <c r="G17" t="s">
         <v>5</v>
       </c>
-      <c r="I17" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>21</v>
+      </c>
       <c r="B18">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -817,9 +838,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>22</v>
+      </c>
       <c r="B19">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -837,9 +861,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>23</v>
+      </c>
       <c r="B20">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C20">
         <v>2</v>

</xml_diff>

<commit_message>
Built out Value cleaning using parsing
The code is still pretty messy, and there are some bugs to fix. The basic flow of logic is established though. Next steps are bug fixing, and some major tidying...
</commit_message>
<xml_diff>
--- a/regex_cases_logic.xlsx
+++ b/regex_cases_logic.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthew.mcfahn/Documents/GitHub/who-api-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE63659F-AE81-E746-ABC5-BF779646A361}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5846A361-508D-0B4A-A33E-7E8771882026}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20400" yWindow="4020" windowWidth="14720" windowHeight="14200" xr2:uid="{D1EB1906-1AF6-C14E-A441-E2525BF29D30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$G$21</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="13">
   <si>
     <t>Cases</t>
   </si>
@@ -450,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A9C09BF-1A38-5B41-9714-1AF4B5C2B4FD}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -516,36 +519,36 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
         <v>3</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -556,90 +559,105 @@
       <c r="F5" t="s">
         <v>6</v>
       </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
         <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
         <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
         <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>5</v>
-      </c>
       <c r="F9" t="s">
         <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -662,24 +680,30 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -702,13 +726,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -719,39 +743,33 @@
       <c r="F13" t="s">
         <v>6</v>
       </c>
-      <c r="G13" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F14" t="s">
         <v>5</v>
-      </c>
-      <c r="G14" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B15">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -763,41 +781,35 @@
         <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>5</v>
-      </c>
-      <c r="G15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" t="s">
         <v>5</v>
       </c>
       <c r="G16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B17">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -806,9 +818,6 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" t="s">
         <v>5</v>
       </c>
       <c r="G17" t="s">
@@ -817,10 +826,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B18">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -829,62 +838,84 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F19" t="s">
         <v>5</v>
       </c>
       <c r="G19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F20" t="s">
         <v>5</v>
       </c>
       <c r="G20" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:G21" xr:uid="{7F2267FF-03F7-5844-AA4C-BFE74BC57F26}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G21">
+      <sortCondition ref="B2:B21"/>
+    </sortState>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="E1:G1"/>
   </mergeCells>

</xml_diff>